<commit_message>
Adding Test Case Results (Fundamental, Api)
</commit_message>
<xml_diff>
--- a/Testcases/TC_05_ADD_PET_API (2.1).xlsx
+++ b/Testcases/TC_05_ADD_PET_API (2.1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Class12Capstone\Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9A8FF77-3E44-43D6-BB32-D3437C97DE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB569CC-0E7C-4EE8-9BEA-9527B8AAD756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11F3F9ED-8A41-4A14-9021-909452B47BB9}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>The example value text should move to the left side of the website into the "parameter value" box</t>
   </si>
   <si>
-    <t xml:space="preserve">5. In the top portion of the "example value" box enter a pet id #, in the bottom portion of it enter what pet type you wish to create. Once you have completed this click the "Try it out!" button at the bottom of the response messages. </t>
-  </si>
-  <si>
     <t>After clicking "Try it out!" the website should give you a 201 response code letting you know that the pet type has been created.</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">If the pet was correctly created earlier the website should display a 200 status response code and the information of the pet type you just requested. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. In the top portion of the "example value" box enter a pet id #, in the bottom portion of it enter "Anaconda" as the pet type you wish to create. Once you have completed this click the "Try it out!" button at the bottom of the response messages. </t>
   </si>
 </sst>
 </file>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B93BE2-F4E8-48E6-B0FC-F4A9C2026B51}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,10 +702,10 @@
     <row r="16" spans="1:5" ht="86.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>19</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -713,10 +713,10 @@
     <row r="17" spans="1:5" ht="59.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -724,10 +724,10 @@
     <row r="18" spans="1:5" ht="58.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>

</xml_diff>